<commit_message>
tested with PyPSA 0.31.0
</commit_message>
<xml_diff>
--- a/scenarios_and_results/Scenario_low_discount_bio_A_par_DAChigh3_biohigh3.xlsx
+++ b/scenarios_and_results/Scenario_low_discount_bio_A_par_DAChigh3_biohigh3.xlsx
@@ -637,10 +637,10 @@
         <v>24</v>
       </c>
       <c r="B2">
-        <v>4274.745549980664</v>
+        <v>4274.745549980666</v>
       </c>
       <c r="C2">
-        <v>1.196928753994586</v>
+        <v>1.196928753994587</v>
       </c>
       <c r="D2">
         <v>7.909628591254097</v>
@@ -649,13 +649,13 @@
         <v>7.909628591254097</v>
       </c>
       <c r="F2">
-        <v>0.08423038439695969</v>
+        <v>0.08423038439695972</v>
       </c>
       <c r="G2">
         <v>7.909628591254096E-05</v>
       </c>
       <c r="H2">
-        <v>0.08430948068287224</v>
+        <v>0.08430948068287226</v>
       </c>
       <c r="I2">
         <v>7.909628591254096E-05</v>
@@ -664,7 +664,7 @@
         <v>7.909628591254097</v>
       </c>
       <c r="K2">
-        <v>0.08430948068287224</v>
+        <v>0.08430948068287226</v>
       </c>
       <c r="L2">
         <v>0.6201859481717517</v>
@@ -673,13 +673,13 @@
         <v>10.65909476155374</v>
       </c>
       <c r="N2">
-        <v>0.211223247726429</v>
+        <v>0.2112232477264289</v>
       </c>
       <c r="O2">
-        <v>0.211223247726429</v>
+        <v>0.2112232477264289</v>
       </c>
       <c r="P2">
-        <v>0.08430948068276434</v>
+        <v>0.08430948068276437</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -703,7 +703,7 @@
         <v>3.38508747542297</v>
       </c>
       <c r="X2">
-        <v>4.524541115831125</v>
+        <v>4.524541115831127</v>
       </c>
       <c r="Y2">
         <v>0</v>
@@ -818,13 +818,13 @@
         <v>0.2380406901525907</v>
       </c>
       <c r="P4">
-        <v>0.1494204170669805</v>
+        <v>0.1494204170669803</v>
       </c>
       <c r="Q4">
         <v>0</v>
       </c>
       <c r="R4">
-        <v>30.84641855071476</v>
+        <v>30.84641855071472</v>
       </c>
       <c r="S4">
         <v>30.84641855073735</v>
@@ -839,10 +839,10 @@
         <v>0</v>
       </c>
       <c r="W4">
-        <v>3.416651432521193</v>
+        <v>3.416651432521195</v>
       </c>
       <c r="X4">
-        <v>1.427360419983422</v>
+        <v>1.42736041998342</v>
       </c>
       <c r="Y4">
         <v>0</v>
@@ -924,13 +924,13 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>0.1510576368333625</v>
+        <v>0.1510576368333628</v>
       </c>
       <c r="F6">
         <v>0.01132094649734388</v>
       </c>
       <c r="G6">
-        <v>0.0006797593657501312</v>
+        <v>0.0006797593657501326</v>
       </c>
       <c r="H6">
         <v>0.01200070586309401</v>
@@ -954,37 +954,37 @@
         <v>0</v>
       </c>
       <c r="O6">
-        <v>0.04812442860818363</v>
+        <v>0.04812442860818372</v>
       </c>
       <c r="P6">
-        <v>0.03482396940101991</v>
+        <v>0.03482396940102008</v>
       </c>
       <c r="Q6">
-        <v>0.02282326353791895</v>
+        <v>0.02282326353791908</v>
       </c>
       <c r="R6">
-        <v>230.5343187609612</v>
+        <v>230.5343187609619</v>
       </c>
       <c r="S6">
-        <v>230.5343187609152</v>
+        <v>230.5343187609156</v>
       </c>
       <c r="T6">
-        <v>74.94454921092439</v>
+        <v>74.94454921092424</v>
       </c>
       <c r="U6">
-        <v>4.499999999999999</v>
+        <v>4.5</v>
       </c>
       <c r="V6">
-        <v>151.0897695499908</v>
+        <v>151.0897695499914</v>
       </c>
       <c r="W6">
-        <v>0.1510576368333625</v>
+        <v>0.1510576368333628</v>
       </c>
       <c r="X6">
         <v>0</v>
       </c>
       <c r="Y6">
-        <v>0.1510576368333625</v>
+        <v>0.1510576368333628</v>
       </c>
     </row>
     <row r="7" spans="1:25">
@@ -1315,7 +1315,7 @@
         <v>52</v>
       </c>
       <c r="B4">
-        <v>2.311001860900218</v>
+        <v>2.311001860900214</v>
       </c>
       <c r="C4">
         <v>0.9488943069551056</v>
@@ -1324,7 +1324,7 @@
         <v>0.948894306955498</v>
       </c>
       <c r="E4">
-        <v>119.9733845119253</v>
+        <v>119.973384511925</v>
       </c>
       <c r="F4">
         <v>15.0633697846841</v>
@@ -1333,37 +1333,37 @@
         <v>15.87465503193345</v>
       </c>
       <c r="H4">
-        <v>1.807203455223223</v>
+        <v>1.807203455223219</v>
       </c>
       <c r="I4">
-        <v>1.807203455223223</v>
+        <v>1.807203455223219</v>
       </c>
       <c r="J4">
-        <v>0.0780884125805027</v>
+        <v>0.07808841258050273</v>
       </c>
       <c r="K4">
-        <v>0.001807203455223222</v>
+        <v>0.001807203455223219</v>
       </c>
       <c r="L4">
-        <v>0.07989561603572592</v>
+        <v>0.07989561603572594</v>
       </c>
       <c r="M4">
-        <v>0.02629384300871606</v>
+        <v>0.02629384300871557</v>
       </c>
       <c r="N4">
-        <v>0.1061894590444501</v>
+        <v>0.1061894590444496</v>
       </c>
       <c r="O4">
-        <v>1.807203455223223</v>
+        <v>1.807203455223219</v>
       </c>
       <c r="P4">
-        <v>58.75899514110084</v>
+        <v>58.75899514110069</v>
       </c>
       <c r="Q4">
-        <v>0.278021478141444</v>
+        <v>0.2780214781414436</v>
       </c>
       <c r="R4">
-        <v>0.2174127959064294</v>
+        <v>0.2174127959064289</v>
       </c>
       <c r="S4">
         <v>1.808843230038229</v>
@@ -1372,19 +1372,19 @@
         <v>1.008978294471503</v>
       </c>
       <c r="U4">
-        <v>0.7998649355667258</v>
+        <v>0.799864935566726</v>
       </c>
       <c r="V4">
-        <v>58.75899514110534</v>
+        <v>58.75899514110517</v>
       </c>
       <c r="W4">
-        <v>43.20953036848712</v>
+        <v>43.20953036848722</v>
       </c>
       <c r="X4">
         <v>1</v>
       </c>
       <c r="Y4">
-        <v>14.54946477261371</v>
+        <v>14.54946477261347</v>
       </c>
     </row>
     <row r="5" spans="1:25">
@@ -1392,10 +1392,10 @@
         <v>53</v>
       </c>
       <c r="B5">
-        <v>3.5680834033479</v>
+        <v>3.568083403347904</v>
       </c>
       <c r="C5">
-        <v>0.8616080904495207</v>
+        <v>0.8616080904495208</v>
       </c>
       <c r="D5">
         <v>0.6375899869326453</v>
@@ -1425,22 +1425,22 @@
         <v>0.03236124562575766</v>
       </c>
       <c r="M5">
-        <v>0.03132075702132643</v>
+        <v>0.03132075702132679</v>
       </c>
       <c r="N5">
-        <v>0.06368200264706271</v>
+        <v>0.06368200264706304</v>
       </c>
       <c r="O5">
-        <v>2.640381718477446</v>
+        <v>2.640381718477448</v>
       </c>
       <c r="P5">
-        <v>24.11848340012208</v>
+        <v>24.11848340012219</v>
       </c>
       <c r="Q5">
-        <v>0.4727386633413331</v>
+        <v>0.4727386633413337</v>
       </c>
       <c r="R5">
-        <v>0.4727386633413331</v>
+        <v>0.4727386633413336</v>
       </c>
       <c r="S5">
         <v>0.3877236407022843</v>
@@ -1452,16 +1452,16 @@
         <v>0</v>
       </c>
       <c r="V5">
-        <v>24.11848340011398</v>
+        <v>24.11848340011409</v>
       </c>
       <c r="W5">
-        <v>12.25627544657388</v>
+        <v>12.25627544657387</v>
       </c>
       <c r="X5">
         <v>0</v>
       </c>
       <c r="Y5">
-        <v>11.8622079535482</v>
+        <v>11.86220795354833</v>
       </c>
     </row>
     <row r="6" spans="1:25">
@@ -1469,22 +1469,22 @@
         <v>54</v>
       </c>
       <c r="B6">
-        <v>0.05275611659207678</v>
+        <v>0.05275611659207704</v>
       </c>
       <c r="C6">
-        <v>0.3689323933590696</v>
+        <v>0.3689323933590697</v>
       </c>
       <c r="D6">
         <v>0.3121919785785857</v>
       </c>
       <c r="E6">
-        <v>23.48889421393267</v>
+        <v>23.48889421393277</v>
       </c>
       <c r="F6">
-        <v>44.9200512476948</v>
+        <v>44.92005124769459</v>
       </c>
       <c r="G6">
-        <v>143.8859878854556</v>
+        <v>143.8859878854549</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -1493,52 +1493,52 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>0.01147241991835246</v>
+        <v>0.01147241991835241</v>
       </c>
       <c r="K6">
         <v>0</v>
       </c>
       <c r="L6">
-        <v>0.01147241991835246</v>
+        <v>0.01147241991835241</v>
       </c>
       <c r="M6">
-        <v>0.02917063331214936</v>
+        <v>0.02917063331215016</v>
       </c>
       <c r="N6">
-        <v>0.04064305323050383</v>
+        <v>0.04064305323050373</v>
       </c>
       <c r="O6">
         <v>1.055122331841537</v>
       </c>
       <c r="P6">
-        <v>38.51975453838254</v>
+        <v>38.51975453838325</v>
       </c>
       <c r="Q6">
-        <v>0.3428003200363145</v>
+        <v>0.3428003200363161</v>
       </c>
       <c r="R6">
         <v>0.3858130991219936</v>
       </c>
       <c r="S6">
-        <v>0.1234619462867746</v>
+        <v>0.123461946286774</v>
       </c>
       <c r="T6">
         <v>0.002177807917998588</v>
       </c>
       <c r="U6">
-        <v>0.121284138368776</v>
+        <v>0.1212841383687754</v>
       </c>
       <c r="V6">
-        <v>38.51975453838445</v>
+        <v>38.51975453838435</v>
       </c>
       <c r="W6">
-        <v>10.87307089627162</v>
+        <v>10.87307089627157</v>
       </c>
       <c r="X6">
         <v>0</v>
       </c>
       <c r="Y6">
-        <v>27.64668364211093</v>
+        <v>27.64668364211168</v>
       </c>
     </row>
     <row r="7" spans="1:25">
@@ -1549,7 +1549,7 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>0.06219197857858567</v>
+        <v>0.06219197857858569</v>
       </c>
       <c r="D7">
         <v>0.8333060567366627</v>
@@ -1558,10 +1558,10 @@
         <v>2.206442658766005</v>
       </c>
       <c r="F7">
-        <v>159.214121631209</v>
+        <v>159.2141216312093</v>
       </c>
       <c r="G7">
-        <v>191.0631998220589</v>
+        <v>191.0631998220593</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -1570,31 +1570,31 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>0.002295483631180213</v>
+        <v>0.002295483631180214</v>
       </c>
       <c r="K7">
         <v>0</v>
       </c>
       <c r="L7">
-        <v>0.002295483631180213</v>
+        <v>0.002295483631180214</v>
       </c>
       <c r="M7">
-        <v>0.02052777990831169</v>
+        <v>0.02052777990831168</v>
       </c>
       <c r="N7">
-        <v>0.02282326353792088</v>
+        <v>0.02282326353792102</v>
       </c>
       <c r="O7">
-        <v>0.3512968298450588</v>
+        <v>0.3512968298450596</v>
       </c>
       <c r="P7">
-        <v>64.96860091096812</v>
+        <v>64.96860091096795</v>
       </c>
       <c r="Q7">
-        <v>0.8266892187292441</v>
+        <v>0.8266892187292433</v>
       </c>
       <c r="R7">
-        <v>0.04812442860818769</v>
+        <v>0.0481244286081878</v>
       </c>
       <c r="S7">
         <v>0.0233127520038915</v>
@@ -1606,16 +1606,16 @@
         <v>0</v>
       </c>
       <c r="V7">
-        <v>64.96860090649608</v>
+        <v>64.96860090649632</v>
       </c>
       <c r="W7">
-        <v>6.534313538191185</v>
+        <v>6.534313538191173</v>
       </c>
       <c r="X7">
         <v>0</v>
       </c>
       <c r="Y7">
-        <v>58.43428737277694</v>
+        <v>58.43428737277678</v>
       </c>
     </row>
     <row r="8" spans="1:25">
@@ -1623,10 +1623,10 @@
         <v>56</v>
       </c>
       <c r="B8">
-        <v>0.006966059038093931</v>
+        <v>0.006966059038093895</v>
       </c>
       <c r="C8">
-        <v>0.0008068171227813768</v>
+        <v>0.0008068171227813769</v>
       </c>
       <c r="D8">
         <v>0.002881489724219203</v>
@@ -1647,52 +1647,52 @@
         <v>0</v>
       </c>
       <c r="J8">
-        <v>0.004078969588126064</v>
+        <v>0.004078969588126066</v>
       </c>
       <c r="K8">
         <v>0</v>
       </c>
       <c r="L8">
-        <v>0.004078969588126064</v>
+        <v>0.004078969588126066</v>
       </c>
       <c r="M8">
-        <v>0.0009421460095680472</v>
+        <v>0.000942146009567613</v>
       </c>
       <c r="N8">
-        <v>0.005021115597693802</v>
+        <v>0.005021115597693779</v>
       </c>
       <c r="O8">
-        <v>0.02487878227890689</v>
+        <v>0.02487878227890676</v>
       </c>
       <c r="P8">
-        <v>201.8232058709397</v>
+        <v>201.8232058709233</v>
       </c>
       <c r="Q8">
-        <v>0.9856164383560971</v>
+        <v>0.9856164383560919</v>
       </c>
       <c r="R8">
-        <v>0.9856164383560969</v>
+        <v>0.9856164383560917</v>
       </c>
       <c r="S8">
-        <v>0.00968180547337652</v>
+        <v>0.009681805473376522</v>
       </c>
       <c r="T8">
-        <v>0.00968180547337652</v>
+        <v>0.009681805473376522</v>
       </c>
       <c r="U8">
         <v>0</v>
       </c>
       <c r="V8">
-        <v>201.8232058709272</v>
+        <v>201.8232058709273</v>
       </c>
       <c r="W8">
-        <v>163.9537475105588</v>
+        <v>163.9537475105597</v>
       </c>
       <c r="X8">
         <v>0</v>
       </c>
       <c r="Y8">
-        <v>37.86945836038092</v>
+        <v>37.86945836036366</v>
       </c>
     </row>
     <row r="9" spans="1:25">
@@ -1700,13 +1700,13 @@
         <v>57</v>
       </c>
       <c r="B9">
-        <v>0.01309409593625981</v>
+        <v>0.01309409593625974</v>
       </c>
       <c r="C9">
         <v>0.001516573539062103</v>
       </c>
       <c r="D9">
-        <v>0.004322234586326993</v>
+        <v>0.004322234586326994</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -1727,49 +1727,49 @@
         <v>0.0002101699747550797</v>
       </c>
       <c r="K9">
-        <v>0.0001164327010652222</v>
+        <v>0.0001164327010652216</v>
       </c>
       <c r="L9">
-        <v>0.0003266026758203019</v>
+        <v>0.0003266026758203014</v>
       </c>
       <c r="M9">
-        <v>0.0004017906878245812</v>
+        <v>0.0004017906878242708</v>
       </c>
       <c r="N9">
-        <v>0.0007283933636448675</v>
+        <v>0.0007283933636445985</v>
       </c>
       <c r="O9">
-        <v>0.03731817341834046</v>
+        <v>0.03731817341834025</v>
       </c>
       <c r="P9">
-        <v>19.51846237165792</v>
+        <v>19.5184623716497</v>
       </c>
       <c r="Q9">
-        <v>0.9856164383559843</v>
+        <v>0.9856164383559791</v>
       </c>
       <c r="R9">
-        <v>0.9856164383559848</v>
+        <v>0.985616438355979</v>
       </c>
       <c r="S9">
-        <v>0.003025564210428895</v>
+        <v>0.003025564210428896</v>
       </c>
       <c r="T9">
-        <v>0.003025564210428895</v>
+        <v>0.003025564210428896</v>
       </c>
       <c r="U9">
         <v>0</v>
       </c>
       <c r="V9">
-        <v>19.5184623716575</v>
+        <v>19.5184623716504</v>
       </c>
       <c r="W9">
-        <v>5.63183981163958</v>
+        <v>5.631839811639611</v>
       </c>
       <c r="X9">
-        <v>3.12</v>
+        <v>3.120000000000001</v>
       </c>
       <c r="Y9">
-        <v>10.76662256001834</v>
+        <v>10.76662256001008</v>
       </c>
     </row>
     <row r="10" spans="1:25">
@@ -1780,7 +1780,7 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <v>-2.531308496146369E-15</v>
+        <v>5.992305578346843E-15</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1807,19 +1807,19 @@
         <v>0</v>
       </c>
       <c r="M10">
-        <v>-5.352793467348316E-16</v>
+        <v>-1.141438766496987E-15</v>
       </c>
       <c r="N10">
-        <v>-5.378238671526731E-16</v>
+        <v>-1.144046496938472E-15</v>
       </c>
       <c r="O10">
-        <v>-2.573473021985552E-15</v>
+        <v>-5.458191578077776E-15</v>
       </c>
       <c r="P10">
         <v>0</v>
       </c>
       <c r="Q10">
-        <v>0.115359406511261</v>
+        <v>-0.10367631670295</v>
       </c>
       <c r="R10" t="s">
         <v>59</v>
@@ -1834,7 +1834,7 @@
         <v>0</v>
       </c>
       <c r="V10">
-        <v>208.9875676014344</v>
+        <v>209.6017482298365</v>
       </c>
       <c r="W10">
         <v>-0</v>
@@ -1843,7 +1843,7 @@
         <v>-0</v>
       </c>
       <c r="Y10">
-        <v>207.9988180027001</v>
+        <v>209.1239836801349</v>
       </c>
     </row>
   </sheetData>

</xml_diff>